<commit_message>
Update fourth spring backlog
</commit_message>
<xml_diff>
--- a/docs/process/sprint-4-backlog.xlsx
+++ b/docs/process/sprint-4-backlog.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12480"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sprint 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="lNSLqQSkb20MMZP0nj+rvd2fhHuqZu3EbfyN1MEuddY="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Remaining effort at the end of the day ...</t>
   </si>
@@ -52,6 +54,9 @@
     <t>Artegiani</t>
   </si>
   <si>
+    <t>/</t>
+  </si>
+  <si>
     <t>Compilazione parametri iniziali</t>
   </si>
   <si>
@@ -61,721 +66,83 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="9">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
-  <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -965,35 +332,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.0857142857143" customWidth="1"/>
-    <col min="2" max="2" width="65.9047619047619" customWidth="1"/>
-    <col min="3" max="3" width="12.6285714285714" customWidth="1"/>
-    <col min="4" max="11" width="5.45714285714286" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="19.38"/>
+    <col customWidth="1" min="2" max="2" width="57.63"/>
+    <col customWidth="1" min="3" max="3" width="11.0"/>
+    <col customWidth="1" min="4" max="11" width="4.75"/>
+    <col customWidth="1" min="12" max="26" width="11.0"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="4:4">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:11">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1007,28 +372,28 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>2.0</v>
       </c>
       <c r="G2" s="1">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="H2" s="1">
-        <v>4</v>
+        <v>4.0</v>
       </c>
       <c r="I2" s="1">
-        <v>5</v>
+        <v>5.0</v>
       </c>
       <c r="J2" s="1">
-        <v>6</v>
+        <v>6.0</v>
       </c>
       <c r="K2" s="1">
-        <v>7</v>
+        <v>7.0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:5">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1039,11 +404,11 @@
         <v>7</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="2:5">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1051,12 +416,12 @@
         <v>7</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:6">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1066,89 +431,116 @@
         <v>11</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" spans="2:5">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:7">
-      <c r="A7" s="3"/>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="4"/>
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="4"/>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1" spans="2:5">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1" spans="4:6">
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A11" s="1"/>
-      <c r="D11" s="1"/>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1" spans="2:4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2134,7 +1526,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>